<commit_message>
Some changes, long time no commit
</commit_message>
<xml_diff>
--- a/2016_07_projects/reference_data.xlsx
+++ b/2016_07_projects/reference_data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16485" windowHeight="7245" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16485" windowHeight="4845"/>
   </bookViews>
   <sheets>
     <sheet name="summary" sheetId="3" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="duval2003coupling" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="222">
   <si>
     <t>a</t>
   </si>
@@ -529,13 +530,195 @@
   </si>
   <si>
     <t>m / ng cm^-2</t>
+  </si>
+  <si>
+    <t>mesh refinement at bpe edges</t>
+  </si>
+  <si>
+    <t>beinning with DeltaPHI=1.4 results not physical</t>
+  </si>
+  <si>
+    <t>error in boundary current flux constraint, OTHER RESULTS TO BE CHECKED</t>
+  </si>
+  <si>
+    <t>error in boundary flux constraint</t>
+  </si>
+  <si>
+    <t>28/07/2016</t>
+  </si>
+  <si>
+    <t>mesh comment</t>
+  </si>
+  <si>
+    <t>result comment 1</t>
+  </si>
+  <si>
+    <t>result comment 2</t>
+  </si>
+  <si>
+    <t>date started</t>
+  </si>
+  <si>
+    <t>project name</t>
+  </si>
+  <si>
+    <t>case comment</t>
+  </si>
+  <si>
+    <t>preparation notes</t>
+  </si>
+  <si>
+    <t>done, domain decomposition solver, regular grid export</t>
+  </si>
+  <si>
+    <t>fine mesh, copied</t>
+  </si>
+  <si>
+    <t>finsih date</t>
+  </si>
+  <si>
+    <t>2016_07_24_15_43_18_tcd2dZNC_duval2003coupling</t>
+  </si>
+  <si>
+    <t>done, domain composition solver, regular grid export both already set up earlier</t>
+  </si>
+  <si>
+    <r>
+      <t>done, domain decomposition solver, fine grid copied earlier, regular grid export, distributed sweep,</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> comsolclusterbatch</t>
+    </r>
+  </si>
+  <si>
+    <t>Wbpe / m</t>
+  </si>
+  <si>
+    <t>Wgap / m</t>
+  </si>
+  <si>
+    <t>DNap</t>
+  </si>
+  <si>
+    <t>DClO4m</t>
+  </si>
+  <si>
+    <t>DeltaX / mm</t>
+  </si>
+  <si>
+    <t>extrapolated to feeder electrodes at W</t>
+  </si>
+  <si>
+    <t>W / m</t>
+  </si>
+  <si>
+    <t>DDSm</t>
+  </si>
+  <si>
+    <t>kappa</t>
+  </si>
+  <si>
+    <t>current density i / A m^-2</t>
+  </si>
+  <si>
+    <t>A / m^2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">speaks for a an area of 50 to 60 cm^2 </t>
+  </si>
+  <si>
+    <t>comparable to duval2003faradaic case b with kappa = 1.4e-1</t>
+  </si>
+  <si>
+    <t>use same kinetic parameters</t>
+  </si>
+  <si>
+    <t>zhang2015control</t>
+  </si>
+  <si>
+    <t>2016_08_01_20_17_50_tertiaryCurrentdDistribution2d_zhang2015control_coarseMesh</t>
+  </si>
+  <si>
+    <t>results are a mess</t>
+  </si>
+  <si>
+    <t>2016_08_01_20_17_50_tertiaryCurrentdDistribution2d_zhang2015control_fineMesh</t>
+  </si>
+  <si>
+    <t>results seem good</t>
+  </si>
+  <si>
+    <t>ran DeltaPHI=1.0 on desktop, took 3 to 4 days</t>
+  </si>
+  <si>
+    <t>2016_08_04_18_42_40_tcd2dZNC_zhang2015control</t>
+  </si>
+  <si>
+    <t>fine Mesh, direct Solver</t>
+  </si>
+  <si>
+    <t>wrong diffusivity parameter found</t>
+  </si>
+  <si>
+    <t>2016_08_05_13_13_07_pde1d_zhang2015control</t>
+  </si>
+  <si>
+    <t>seems to be stuck at 4th solver step</t>
+  </si>
+  <si>
+    <t>does not converge at DeltaPHI = 1 V</t>
+  </si>
+  <si>
+    <t>server</t>
+  </si>
+  <si>
+    <t>location</t>
+  </si>
+  <si>
+    <t>no physical results, always some c &lt;0</t>
+  </si>
+  <si>
+    <t>seems ok, except single "ausreisser"</t>
+  </si>
+  <si>
+    <t>direct solver, regular grid export</t>
+  </si>
+  <si>
+    <t>done, domain decomposition solver set up earlier already, regular grid export, sweep set back to full range, comsolclusterbatch</t>
+  </si>
+  <si>
+    <t>direct solver, regular grid export, full range</t>
+  </si>
+  <si>
+    <t>done, domain decomposition solver, regular grid export, distributed sweep</t>
+  </si>
+  <si>
+    <t>error in background electrolyte concentration</t>
+  </si>
+  <si>
+    <t>2016_07_17_19_13_49_tcd2dZNC_duval2003faradaic_case_d_direct</t>
+  </si>
+  <si>
+    <t>direct solver</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
+    <numFmt numFmtId="165" formatCode="0.0000E+00"/>
+  </numFmts>
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -551,13 +734,45 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -569,19 +784,28 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Bad" xfId="1" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -612,7 +836,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1174,7 +1397,6 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -1319,7 +1541,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1401,7 +1622,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1442,7 +1662,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>zhang2015control!$B$34</c:f>
+              <c:f>zhang2015control!$B$39</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1475,7 +1695,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>zhang2015control!$B$36:$B$54</c:f>
+              <c:f>zhang2015control!$B$41:$B$59</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="19"/>
@@ -1541,7 +1761,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>zhang2015control!$C$36:$C$54</c:f>
+              <c:f>zhang2015control!$C$41:$C$59</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="19"/>
@@ -1617,7 +1837,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>zhang2015control!$D$34</c:f>
+              <c:f>zhang2015control!$D$39</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1650,7 +1870,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>zhang2015control!$D$36:$D$54</c:f>
+              <c:f>zhang2015control!$D$41:$D$59</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="19"/>
@@ -1713,7 +1933,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>zhang2015control!$E$36:$E$54</c:f>
+              <c:f>zhang2015control!$E$41:$E$59</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="19"/>
@@ -1786,7 +2006,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>zhang2015control!$F$34</c:f>
+              <c:f>zhang2015control!$F$39</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1819,7 +2039,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>zhang2015control!$F$36:$F$54</c:f>
+              <c:f>zhang2015control!$F$41:$F$59</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="19"/>
@@ -1885,7 +2105,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>zhang2015control!$G$36:$G$54</c:f>
+              <c:f>zhang2015control!$G$41:$G$59</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="19"/>
@@ -2101,7 +2321,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2183,6 +2402,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3149,6 +3369,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3230,6 +3451,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4090,6 +4312,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4769,6 +4992,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6321,6 +6545,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7537,6 +7762,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -8278,6 +8504,7 @@
           </c:spPr>
         </c:majorGridlines>
         <c:title>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -8370,6 +8597,7 @@
           </c:spPr>
         </c:majorGridlines>
         <c:title>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -8450,6 +8678,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -13762,13 +13991,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:row>44</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>54</xdr:row>
+      <xdr:row>59</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -14276,26 +14505,62 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I24"/>
+  <dimension ref="A1:L43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="19.5703125" customWidth="1"/>
     <col min="3" max="3" width="7.7109375" customWidth="1"/>
-    <col min="4" max="4" width="77" customWidth="1"/>
-    <col min="5" max="5" width="23.140625" customWidth="1"/>
+    <col min="4" max="5" width="77" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="10.7109375" style="8" customWidth="1"/>
+    <col min="9" max="9" width="33.140625" customWidth="1"/>
+    <col min="10" max="10" width="36.5703125" customWidth="1"/>
+    <col min="11" max="11" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>177</v>
+      </c>
+      <c r="D2" t="s">
+        <v>176</v>
+      </c>
+      <c r="E2" t="s">
+        <v>178</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>212</v>
+      </c>
+      <c r="I2" t="s">
+        <v>172</v>
+      </c>
+      <c r="J2" t="s">
+        <v>173</v>
+      </c>
+      <c r="K2" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>95</v>
       </c>
@@ -14305,161 +14570,498 @@
       <c r="D4" t="s">
         <v>97</v>
       </c>
-      <c r="F4" s="6">
+      <c r="F4" s="8">
         <v>42563</v>
       </c>
-      <c r="G4" t="s">
+      <c r="J4" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>103</v>
       </c>
       <c r="D5" t="s">
         <v>123</v>
       </c>
-      <c r="E5" t="s">
+      <c r="I5" t="s">
         <v>137</v>
       </c>
-      <c r="F5" s="6"/>
-      <c r="G5" t="s">
+      <c r="J5" t="s">
         <v>131</v>
       </c>
-      <c r="H5" t="s">
+      <c r="K5" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D6" t="s">
+    <row r="6" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D6" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" s="9">
+        <v>42565</v>
+      </c>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="F6" s="6">
-        <v>42565</v>
-      </c>
-      <c r="H6" t="s">
+      <c r="J6" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="K6" s="6" t="s">
         <v>144</v>
       </c>
-      <c r="I6" t="s">
+      <c r="L6" s="6" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D7" t="s">
         <v>154</v>
       </c>
-      <c r="F7" s="6">
+      <c r="F7" s="8">
         <v>42569</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
+    <row r="8" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D8" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="G8" s="9">
+        <v>42583</v>
+      </c>
+      <c r="H8" s="9"/>
+      <c r="I8" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="J8" s="9" t="s">
+        <v>213</v>
+      </c>
+      <c r="K8" s="6" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>133</v>
+      </c>
+      <c r="E9" t="s">
+        <v>215</v>
+      </c>
+      <c r="F9" s="8">
+        <v>42592</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="J9" s="8"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J10" s="8"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
         <v>135</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D11" t="s">
         <v>138</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F11" s="8">
+        <v>42566</v>
+      </c>
+      <c r="I11" t="s">
         <v>139</v>
       </c>
-      <c r="F9" s="6">
+      <c r="J11" t="s">
+        <v>140</v>
+      </c>
+      <c r="K11" t="s">
+        <v>150</v>
+      </c>
+      <c r="L11" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D12" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="6" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D13" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="F13" s="9">
+        <v>42579</v>
+      </c>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9" t="s">
+        <v>211</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="J13" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="K13" s="6" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D14" t="s">
+        <v>151</v>
+      </c>
+      <c r="E14" t="s">
+        <v>217</v>
+      </c>
+      <c r="F14" s="8">
+        <v>42592</v>
+      </c>
+      <c r="H14" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="I14" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="F16" s="9">
         <v>42566</v>
       </c>
-      <c r="G9" t="s">
-        <v>140</v>
-      </c>
-      <c r="H9" t="s">
-        <v>150</v>
-      </c>
-      <c r="I9" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D10" t="s">
-        <v>151</v>
-      </c>
-      <c r="E10" t="s">
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="6" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>136</v>
-      </c>
-      <c r="D13" t="s">
+      <c r="J16" s="6" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D17" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F17" s="10">
+        <v>42578</v>
+      </c>
+      <c r="G17" s="10"/>
+      <c r="H17" s="10"/>
+      <c r="I17" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="J17" s="7" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D18" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="F13" s="6">
-        <v>42566</v>
-      </c>
-      <c r="G13" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D14" t="s">
+    </row>
+    <row r="19" spans="2:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D19" s="6" t="s">
         <v>152</v>
       </c>
-      <c r="E14" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
+      <c r="F19" s="9">
+        <v>42578</v>
+      </c>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="J19" s="6" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D20" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="F20" s="9">
+        <v>42579</v>
+      </c>
+      <c r="G20" s="9">
+        <v>42583</v>
+      </c>
+      <c r="H20" s="9"/>
+      <c r="I20" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="J20" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="K20" s="6" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="D21" t="s">
+        <v>152</v>
+      </c>
+      <c r="E21" t="s">
+        <v>215</v>
+      </c>
+      <c r="F21" s="8">
+        <v>42592</v>
+      </c>
+      <c r="H21" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="I21" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
         <v>146</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D23" t="s">
         <v>145</v>
       </c>
-      <c r="E17" t="s">
+      <c r="F23" s="8">
+        <v>42568</v>
+      </c>
+      <c r="I23" t="s">
         <v>147</v>
       </c>
-      <c r="F17" s="6">
-        <v>42568</v>
-      </c>
-      <c r="G17" t="s">
+      <c r="J23" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="D18" t="s">
+    <row r="24" spans="2:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D24" s="6" t="s">
         <v>153</v>
       </c>
-      <c r="E18" t="s">
+      <c r="F24" s="9">
+        <v>42574</v>
+      </c>
+      <c r="G24" s="9"/>
+      <c r="H24" s="9"/>
+      <c r="I24" s="6" t="s">
         <v>147</v>
       </c>
-      <c r="F18" s="6">
-        <v>42574</v>
-      </c>
-      <c r="G18" t="s">
+      <c r="J24" s="6" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
+      <c r="K24" s="6" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="D25" t="s">
+        <v>153</v>
+      </c>
+      <c r="E25" t="s">
+        <v>184</v>
+      </c>
+      <c r="F25" s="8">
+        <v>42579</v>
+      </c>
+      <c r="I25" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="D26" t="s">
+        <v>220</v>
+      </c>
+      <c r="E26" t="s">
+        <v>221</v>
+      </c>
+      <c r="I26" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="30" spans="2:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C30" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D30" s="6" t="s">
         <v>157</v>
       </c>
-      <c r="E24" t="s">
+      <c r="F30" s="9">
+        <v>42575</v>
+      </c>
+      <c r="G30" s="9"/>
+      <c r="H30" s="9"/>
+      <c r="I30" s="6" t="s">
         <v>158</v>
       </c>
-      <c r="F24" s="6">
-        <v>42575</v>
-      </c>
-      <c r="G24" t="s">
+      <c r="J30" s="6" t="s">
         <v>159</v>
+      </c>
+    </row>
+    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C31" t="s">
+        <v>96</v>
+      </c>
+      <c r="D31" t="s">
+        <v>157</v>
+      </c>
+      <c r="F31" s="8">
+        <v>42578</v>
+      </c>
+      <c r="G31" s="8">
+        <v>42579</v>
+      </c>
+      <c r="I31" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C32" t="s">
+        <v>96</v>
+      </c>
+      <c r="D32" t="s">
+        <v>182</v>
+      </c>
+      <c r="E32" t="s">
+        <v>183</v>
+      </c>
+      <c r="F32" s="8">
+        <v>42579</v>
+      </c>
+      <c r="I32" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="37" spans="2:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="D37" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="F37" s="9">
+        <v>42583</v>
+      </c>
+      <c r="G37" s="9">
+        <v>42583</v>
+      </c>
+      <c r="H37" s="9"/>
+      <c r="J37" s="6" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="38" spans="2:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D38" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="F38" s="9">
+        <v>42583</v>
+      </c>
+      <c r="G38" s="9">
+        <v>42584</v>
+      </c>
+      <c r="H38" s="9"/>
+      <c r="J38" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="K38" s="6" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="39" spans="2:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D39" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="E39" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="F39" s="9">
+        <v>42587</v>
+      </c>
+      <c r="G39" s="9">
+        <v>42587</v>
+      </c>
+      <c r="H39" s="9"/>
+      <c r="K39" s="6" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="40" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="D40" t="s">
+        <v>202</v>
+      </c>
+      <c r="F40" s="8">
+        <v>42587</v>
+      </c>
+      <c r="G40" s="8">
+        <v>42587</v>
+      </c>
+    </row>
+    <row r="41" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="D41" t="s">
+        <v>205</v>
+      </c>
+      <c r="F41" s="8">
+        <v>42587</v>
+      </c>
+      <c r="G41" s="8">
+        <v>42587</v>
+      </c>
+    </row>
+    <row r="42" spans="2:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D42" s="7" t="s">
+        <v>208</v>
+      </c>
+      <c r="F42" s="10">
+        <v>42588</v>
+      </c>
+      <c r="G42" s="10"/>
+      <c r="H42" s="10"/>
+      <c r="J42" s="7" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="43" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="D43" t="s">
+        <v>208</v>
+      </c>
+      <c r="F43" s="8">
+        <v>42587</v>
+      </c>
+      <c r="G43" s="8">
+        <v>42587</v>
+      </c>
+      <c r="J43" t="s">
+        <v>214</v>
       </c>
     </row>
   </sheetData>
@@ -14470,23 +15072,309 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A8:G54"/>
+  <dimension ref="A1:AA59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="S38" sqref="S38"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="16" max="16" width="11.5703125" customWidth="1"/>
+    <col min="17" max="17" width="10" style="11" customWidth="1"/>
+    <col min="19" max="19" width="12.28515625" customWidth="1"/>
+    <col min="21" max="21" width="10.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>191</v>
+      </c>
+      <c r="B1" s="1">
+        <f>B3+2*B2</f>
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>44</v>
+      </c>
+      <c r="P1" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q1" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="R1" t="s">
+        <v>75</v>
+      </c>
+      <c r="S1" t="s">
+        <v>77</v>
+      </c>
+      <c r="T1" t="s">
+        <v>81</v>
+      </c>
+      <c r="U1" t="s">
+        <v>90</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>186</v>
+      </c>
+      <c r="B2" s="1">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="O2" s="1">
+        <v>1</v>
+      </c>
+      <c r="P2" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q2" s="11">
+        <v>9.3109999999999998E-9</v>
+      </c>
+      <c r="R2">
+        <v>349.65</v>
+      </c>
+      <c r="S2" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="T2">
+        <v>1</v>
+      </c>
+      <c r="U2" s="1">
+        <f>$AA$2^2/($AA$3*$AA$4)*$T2^2*$Q2*$S2</f>
+        <v>3.496632473739711E-6</v>
+      </c>
+      <c r="V2" s="1"/>
+      <c r="W2" s="1"/>
+      <c r="X2" s="1"/>
+      <c r="Z2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AA2">
+        <v>96485.336500000005</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>185</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3" s="1">
+        <v>1000</v>
+      </c>
+      <c r="G3" s="1">
+        <v>1000</v>
+      </c>
+      <c r="O3" s="1">
+        <v>1</v>
+      </c>
+      <c r="P3" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q3" s="11">
+        <v>5.2730000000000003E-9</v>
+      </c>
+      <c r="R3">
+        <v>198</v>
+      </c>
+      <c r="S3" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="T3">
+        <v>1</v>
+      </c>
+      <c r="U3" s="1">
+        <f>$AA$2^2/($AA$3*$AA$4)*T3^2*Q3*S3</f>
+        <v>1.9802108295596066E-6</v>
+      </c>
+      <c r="V3" s="1"/>
+      <c r="W3" s="1"/>
+      <c r="X3" s="1"/>
+      <c r="Z3" t="s">
+        <v>80</v>
+      </c>
+      <c r="AA3">
+        <v>8.3144621000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="D4" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="E4" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="O4" s="1">
+        <v>1</v>
+      </c>
+      <c r="P4" t="s">
+        <v>192</v>
+      </c>
+      <c r="Q4" s="11">
+        <v>6.3899999999999996E-10</v>
+      </c>
+      <c r="R4">
+        <v>24</v>
+      </c>
+      <c r="S4" s="1">
+        <v>0.15</v>
+      </c>
+      <c r="T4">
+        <v>1</v>
+      </c>
+      <c r="U4" s="1">
+        <f>$AA$2^2/($AA$3*$AA$4)*T4^2*Q4*S4</f>
+        <v>3.5995298314676325E-4</v>
+      </c>
+      <c r="V4" s="1"/>
+      <c r="W4" s="1"/>
+      <c r="X4" s="1"/>
+      <c r="Z4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AA4">
+        <v>298.14999999999998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="D5" s="1">
+        <v>1.4999999999999999E-4</v>
+      </c>
+      <c r="F5" s="1">
+        <f>D5*F3</f>
+        <v>0.15</v>
+      </c>
+      <c r="O5" s="1">
+        <v>1</v>
+      </c>
+      <c r="P5" t="s">
+        <v>187</v>
+      </c>
+      <c r="Q5" s="11">
+        <v>1.3339999999999999E-9</v>
+      </c>
+      <c r="R5">
+        <v>50.08</v>
+      </c>
+      <c r="S5" s="1">
+        <f>S4+S6</f>
+        <v>10.15</v>
+      </c>
+      <c r="T5">
+        <v>1</v>
+      </c>
+      <c r="U5" s="1">
+        <f t="shared" ref="U5:U6" si="0">$AA$2^2/($AA$3*$AA$4)*T5^2*Q5*S5</f>
+        <v>5.0848193918680118E-2</v>
+      </c>
+      <c r="V5" s="1"/>
+      <c r="W5" s="1"/>
+      <c r="X5" s="1"/>
+      <c r="Z5" t="s">
+        <v>83</v>
+      </c>
+      <c r="AA5">
+        <f>AA2/AA3/AA4</f>
+        <v>38.921748687348185</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="O6" s="1"/>
+      <c r="P6" t="s">
+        <v>188</v>
+      </c>
+      <c r="Q6" s="11">
+        <v>1.792E-9</v>
+      </c>
+      <c r="R6">
+        <v>67.3</v>
+      </c>
+      <c r="S6" s="1">
+        <v>10</v>
+      </c>
+      <c r="T6">
+        <v>1</v>
+      </c>
+      <c r="U6" s="1">
+        <f t="shared" si="0"/>
+        <v>6.7296374105268619E-2</v>
+      </c>
+      <c r="V6" s="1"/>
+      <c r="W6" s="1"/>
+      <c r="X6" s="1"/>
+    </row>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="O7" s="1"/>
+      <c r="S7" s="1"/>
+      <c r="U7" s="1"/>
+      <c r="V7" s="1"/>
+      <c r="W7" s="1"/>
+      <c r="X7" s="1"/>
+      <c r="Z7" t="s">
+        <v>87</v>
+      </c>
+      <c r="AA7" s="1">
+        <v>6.0221399999999997E+23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>160</v>
       </c>
       <c r="B8" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="T8" t="s">
+        <v>193</v>
+      </c>
+      <c r="U8" s="1">
+        <f>SUM(U2:U6)</f>
+        <v>0.1185099978503988</v>
+      </c>
+      <c r="V8" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="W8" s="1"/>
+      <c r="X8" s="1"/>
+      <c r="Z8" t="s">
+        <v>88</v>
+      </c>
+      <c r="AA8" s="1">
+        <f>AA2/AA7</f>
+        <v>1.6021769088729256E-19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>161</v>
       </c>
@@ -14499,8 +15387,28 @@
       <c r="F9">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="V9" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10">
+        <f>B9*0.001</f>
+        <v>1E-4</v>
+      </c>
+      <c r="D10">
+        <f t="shared" ref="D10:F10" si="1">D9*0.001</f>
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="1"/>
+        <v>4.0000000000000002E-4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>162</v>
       </c>
@@ -14520,7 +15428,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>0.4996601</v>
       </c>
@@ -14540,7 +15448,7 @@
         <v>269.91986000000003</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>1.006524</v>
       </c>
@@ -14560,7 +15468,7 @@
         <v>233.65827999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B14">
         <v>1.5135567999999999</v>
       </c>
@@ -14580,7 +15488,7 @@
         <v>204.45808</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B15">
         <v>1.9815442999999999</v>
       </c>
@@ -14600,7 +15508,7 @@
         <v>182.33306999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B16">
         <v>2.5145849999999998</v>
       </c>
@@ -14620,7 +15528,7 @@
         <v>156.66759999999999</v>
       </c>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B17">
         <v>2.9956101999999998</v>
       </c>
@@ -14640,7 +15548,7 @@
         <v>133.65575000000001</v>
       </c>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B18">
         <v>3.5156638999999998</v>
       </c>
@@ -14660,7 +15568,7 @@
         <v>109.76050600000001</v>
       </c>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B19">
         <v>3.9966889999999999</v>
       </c>
@@ -14680,7 +15588,7 @@
         <v>84.980720000000005</v>
       </c>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B20">
         <v>4.5037216999999998</v>
       </c>
@@ -14700,7 +15608,7 @@
         <v>61.083182999999998</v>
       </c>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B21">
         <v>5.0107379999999999</v>
       </c>
@@ -14720,7 +15628,7 @@
         <v>38.955874999999999</v>
       </c>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B22">
         <v>5.5178045999999998</v>
       </c>
@@ -14740,7 +15648,7 @@
         <v>15.064076999999999</v>
       </c>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B23">
         <v>6.0248375000000003</v>
       </c>
@@ -14760,7 +15668,7 @@
         <v>-9.7180029999999995</v>
       </c>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B24">
         <v>6.505846</v>
       </c>
@@ -14780,7 +15688,7 @@
         <v>-32.731003000000001</v>
       </c>
     </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B25">
         <v>7.0128789999999999</v>
       </c>
@@ -14800,7 +15708,7 @@
         <v>-56.625095000000002</v>
       </c>
     </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B26">
         <v>7.5199284999999998</v>
       </c>
@@ -14820,7 +15728,7 @@
         <v>-80.520340000000004</v>
       </c>
     </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B27">
         <v>8.0139580000000006</v>
       </c>
@@ -14840,7 +15748,7 @@
         <v>-107.068054</v>
       </c>
     </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B28">
         <v>8.4949320000000004</v>
       </c>
@@ -14860,7 +15768,7 @@
         <v>-128.31198000000001</v>
       </c>
     </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B29">
         <v>9.0019480000000005</v>
       </c>
@@ -14880,7 +15788,7 @@
         <v>-158.39326</v>
       </c>
     </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B30">
         <v>9.5089129999999997</v>
       </c>
@@ -14900,419 +15808,519 @@
         <v>-191.12242000000001</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>189</v>
+      </c>
+      <c r="B32">
+        <f>B30-B12</f>
+        <v>9.0092528999999999</v>
+      </c>
+      <c r="D32">
+        <f t="shared" ref="D32:F32" si="2">D30-D12</f>
+        <v>9.0197376999999985</v>
+      </c>
+      <c r="F32">
+        <f t="shared" si="2"/>
+        <v>8.9898739999999986</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>7</v>
+      </c>
+      <c r="B33">
+        <f>($B$1*1000/B$32)*(C$12-C$30)*0.001</f>
+        <v>0.15628934892037497</v>
+      </c>
+      <c r="D33">
+        <f t="shared" ref="D33:F33" si="3">($B$1/D$32)*(E$12-E$30)</f>
+        <v>0.31663257957046803</v>
+      </c>
+      <c r="F33">
+        <f t="shared" si="3"/>
+        <v>0.56413082986480123</v>
+      </c>
+      <c r="H33" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>194</v>
+      </c>
+      <c r="B34" s="1">
+        <f>$U$8*B$33</f>
+        <v>1.8521850404593865E-2</v>
+      </c>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1">
+        <f t="shared" ref="D34:F34" si="4">$U$8*D$33</f>
+        <v>3.7524126324262393E-2</v>
+      </c>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1">
+        <f t="shared" si="4"/>
+        <v>6.6855143434621289E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>195</v>
+      </c>
+      <c r="B35" s="1">
+        <f>B$10/B$34</f>
+        <v>5.3990285967970885E-3</v>
+      </c>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1">
+        <f t="shared" ref="D35:F35" si="5">D$10/D$34</f>
+        <v>5.3299042400537858E-3</v>
+      </c>
+      <c r="E35" s="1"/>
+      <c r="F35" s="1">
+        <f t="shared" si="5"/>
+        <v>5.9830849123996927E-3</v>
+      </c>
+      <c r="I35" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>16</v>
+      </c>
+      <c r="B36" s="1">
+        <f>SQRT(B$35)</f>
+        <v>7.3478082424605282E-2</v>
+      </c>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1">
+        <f t="shared" ref="D36:F36" si="6">SQRT(D$35)</f>
+        <v>7.3006193162318669E-2</v>
+      </c>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1">
+        <f t="shared" si="6"/>
+        <v>7.7350403440445567E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B37" s="1"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>96</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B38" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>161</v>
       </c>
-      <c r="B34">
+      <c r="B39">
         <v>0.1</v>
       </c>
-      <c r="D34">
+      <c r="D39">
         <v>0.2</v>
       </c>
-      <c r="F34">
+      <c r="F39">
         <v>0.4</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B35" t="s">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
         <v>162</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C40" t="s">
         <v>166</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D40" t="s">
         <v>162</v>
       </c>
-      <c r="E35" t="s">
+      <c r="E40" t="s">
         <v>166</v>
       </c>
-      <c r="F35" t="s">
+      <c r="F40" t="s">
         <v>162</v>
       </c>
-      <c r="G35" t="s">
+      <c r="G40" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B36">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B41">
         <v>0.51329539999999996</v>
       </c>
-      <c r="C36">
+      <c r="C41">
         <v>3.5825553000000001</v>
       </c>
-      <c r="D36">
+      <c r="D41">
         <v>0.50062364000000004</v>
       </c>
-      <c r="E36">
+      <c r="E41">
         <v>2.8105354</v>
       </c>
-      <c r="F36">
+      <c r="F41">
         <v>0.48786934999999998</v>
       </c>
-      <c r="G36">
+      <c r="G41">
         <v>2.3893925999999999</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B37">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B42">
         <v>1.0144808000000001</v>
       </c>
-      <c r="C37">
+      <c r="C42">
         <v>4.0071260000000004</v>
       </c>
-      <c r="D37">
+      <c r="D42">
         <v>1.0403530000000001</v>
       </c>
-      <c r="E37">
+      <c r="E42">
         <v>3.3055517999999999</v>
       </c>
-      <c r="F37">
+      <c r="F42">
         <v>1.0019412000000001</v>
       </c>
-      <c r="G37">
+      <c r="G42">
         <v>2.6737022000000001</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B38">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B43">
         <v>1.5284040000000001</v>
       </c>
-      <c r="C38">
+      <c r="C43">
         <v>4.9230146000000001</v>
       </c>
-      <c r="D38">
+      <c r="D43">
         <v>1.502945</v>
       </c>
-      <c r="E38">
+      <c r="E43">
         <v>3.8702025</v>
       </c>
-      <c r="F38">
+      <c r="F43">
         <v>1.5031432</v>
       </c>
-      <c r="G38">
+      <c r="G43">
         <v>3.0280971999999999</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B39">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B44">
         <v>2.0166037000000001</v>
       </c>
-      <c r="C39">
+      <c r="C44">
         <v>5.9088984</v>
       </c>
-      <c r="D39">
+      <c r="D44">
         <v>2.0040971999999999</v>
       </c>
-      <c r="E39">
+      <c r="E44">
         <v>4.4351240000000001</v>
       </c>
-      <c r="F39">
+      <c r="F44">
         <v>1.9786216000000001</v>
       </c>
-      <c r="G39">
+      <c r="G44">
         <v>3.4524872000000002</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B40">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B45">
         <v>2.5175909999999999</v>
       </c>
-      <c r="C40">
+      <c r="C45">
         <v>7.1755740000000001</v>
       </c>
-      <c r="D40">
+      <c r="D45">
         <v>2.5051339000000001</v>
       </c>
-      <c r="E40">
+      <c r="E45">
         <v>5.4912733999999999</v>
       </c>
-      <c r="F40">
+      <c r="F45">
         <v>2.4925449999999998</v>
       </c>
-      <c r="G40">
+      <c r="G45">
         <v>4.3683759999999996</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B41">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B46">
         <v>2.9927554000000001</v>
       </c>
-      <c r="C41">
+      <c r="C46">
         <v>8.9332969999999996</v>
       </c>
-      <c r="D41">
+      <c r="D46">
         <v>3.0189085000000002</v>
       </c>
-      <c r="E41">
+      <c r="E46">
         <v>7.0387405999999997</v>
       </c>
-      <c r="F41">
+      <c r="F46">
         <v>2.9936311</v>
       </c>
-      <c r="G41">
+      <c r="G46">
         <v>5.2139990000000003</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B42">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B47">
         <v>3.519301</v>
       </c>
-      <c r="C42">
+      <c r="C47">
         <v>10.831733</v>
       </c>
-      <c r="D42">
+      <c r="D47">
         <v>3.5068769999999998</v>
       </c>
-      <c r="E42">
+      <c r="E47">
         <v>9.0070809999999994</v>
       </c>
-      <c r="F42">
+      <c r="F47">
         <v>3.4945520999999999</v>
       </c>
-      <c r="G42">
+      <c r="G47">
         <v>6.7613763999999996</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B43">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B48">
         <v>4.0330424000000002</v>
       </c>
-      <c r="C43">
+      <c r="C48">
         <v>12.519551</v>
       </c>
-      <c r="D43">
+      <c r="D48">
         <v>4.0076327000000003</v>
       </c>
-      <c r="E43">
+      <c r="E48">
         <v>11.256212</v>
       </c>
-      <c r="F43">
+      <c r="F48">
         <v>4.0467715000000002</v>
       </c>
-      <c r="G43">
+      <c r="G48">
         <v>8.8003429999999998</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B44">
-        <v>4.520994</v>
-      </c>
-      <c r="C44">
-        <v>14.558066</v>
-      </c>
-      <c r="D44">
-        <v>4.5083060000000001</v>
-      </c>
-      <c r="E44">
-        <v>13.856221</v>
-      </c>
-      <c r="F44">
-        <v>4.5603147000000002</v>
-      </c>
-      <c r="G44">
-        <v>11.330266999999999</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B45">
-        <v>5.0474569999999996</v>
-      </c>
-      <c r="C45">
-        <v>16.807379000000001</v>
-      </c>
-      <c r="D45">
-        <v>5.0218660000000002</v>
-      </c>
-      <c r="E45">
-        <v>16.31597</v>
-      </c>
-      <c r="F45">
-        <v>5.0096069999999999</v>
-      </c>
-      <c r="G45">
-        <v>13.789564</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B46">
-        <v>5.5354752999999999</v>
-      </c>
-      <c r="C46">
-        <v>18.565190999999999</v>
-      </c>
-      <c r="D46">
-        <v>5.5226709999999999</v>
-      </c>
-      <c r="E46">
-        <v>18.354576000000002</v>
-      </c>
-      <c r="F46">
-        <v>5.5102969999999996</v>
-      </c>
-      <c r="G46">
-        <v>16.319396999999999</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B47">
-        <v>6.0236749999999999</v>
-      </c>
-      <c r="C47">
-        <v>19.551075000000001</v>
-      </c>
-      <c r="D47">
-        <v>5.9978850000000001</v>
-      </c>
-      <c r="E47">
-        <v>19.901772000000001</v>
-      </c>
-      <c r="F47">
-        <v>6.0110029999999997</v>
-      </c>
-      <c r="G47">
-        <v>18.779057000000002</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B48">
-        <v>6.4990873000000002</v>
-      </c>
-      <c r="C48">
-        <v>20.256166</v>
-      </c>
-      <c r="D48">
-        <v>7.0127625</v>
-      </c>
-      <c r="E48">
-        <v>22.224688</v>
-      </c>
-      <c r="F48">
-        <v>6.4988393999999996</v>
-      </c>
-      <c r="G48">
-        <v>21.308800000000002</v>
       </c>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B49">
-        <v>6.9873529999999997</v>
+        <v>4.520994</v>
       </c>
       <c r="C49">
-        <v>20.961349999999999</v>
+        <v>14.558066</v>
       </c>
       <c r="D49">
-        <v>7.5523924999999998</v>
+        <v>4.5083060000000001</v>
       </c>
       <c r="E49">
-        <v>23.140757000000001</v>
+        <v>13.856221</v>
       </c>
       <c r="F49">
-        <v>7.0380893000000002</v>
+        <v>4.5603147000000002</v>
       </c>
       <c r="G49">
-        <v>23.838902999999998</v>
+        <v>11.330266999999999</v>
       </c>
     </row>
     <row r="50" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B50">
-        <v>7.5142455000000004</v>
+        <v>5.0474569999999996</v>
       </c>
       <c r="C50">
-        <v>21.386099999999999</v>
+        <v>16.807379000000001</v>
       </c>
       <c r="D50">
-        <v>8.0277560000000001</v>
+        <v>5.0218660000000002</v>
       </c>
       <c r="E50">
-        <v>24.056376</v>
+        <v>16.31597</v>
       </c>
       <c r="F50">
-        <v>7.5132212999999997</v>
+        <v>5.0096069999999999</v>
       </c>
       <c r="G50">
-        <v>25.736977</v>
+        <v>13.789564</v>
       </c>
     </row>
     <row r="51" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B51">
-        <v>8.0024949999999997</v>
+        <v>5.5354752999999999</v>
       </c>
       <c r="C51">
-        <v>22.161456999999999</v>
+        <v>18.565190999999999</v>
       </c>
       <c r="D51">
-        <v>8.5545819999999999</v>
+        <v>5.5226709999999999</v>
       </c>
       <c r="E51">
-        <v>24.761827</v>
+        <v>18.354576000000002</v>
       </c>
       <c r="F51">
-        <v>8.0269619999999993</v>
+        <v>5.5102969999999996</v>
       </c>
       <c r="G51">
-        <v>27.424795</v>
+        <v>16.319396999999999</v>
       </c>
     </row>
     <row r="52" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B52">
-        <v>8.5165830000000007</v>
+        <v>6.0236749999999999</v>
       </c>
       <c r="C52">
-        <v>22.375591</v>
+        <v>19.551075000000001</v>
       </c>
       <c r="D52">
-        <v>9.0300600000000006</v>
+        <v>5.9978850000000001</v>
       </c>
       <c r="E52">
-        <v>25.186218</v>
+        <v>19.901772000000001</v>
       </c>
       <c r="F52">
-        <v>8.4893730000000005</v>
+        <v>6.0110029999999997</v>
       </c>
       <c r="G52">
-        <v>28.761377</v>
+        <v>18.779057000000002</v>
       </c>
     </row>
     <row r="53" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B53">
-        <v>8.9920950000000008</v>
+        <v>6.4990873000000002</v>
       </c>
       <c r="C53">
-        <v>22.659631999999998</v>
+        <v>20.256166</v>
       </c>
       <c r="D53">
-        <v>9.5440830000000005</v>
+        <v>7.0127625</v>
       </c>
       <c r="E53">
-        <v>25.681052999999999</v>
+        <v>22.224688</v>
       </c>
       <c r="F53">
-        <v>9.0290189999999999</v>
+        <v>6.4988393999999996</v>
       </c>
       <c r="G53">
-        <v>29.60727</v>
+        <v>21.308800000000002</v>
       </c>
     </row>
     <row r="54" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B54">
+        <v>6.9873529999999997</v>
+      </c>
+      <c r="C54">
+        <v>20.961349999999999</v>
+      </c>
+      <c r="D54">
+        <v>7.5523924999999998</v>
+      </c>
+      <c r="E54">
+        <v>23.140757000000001</v>
+      </c>
+      <c r="F54">
+        <v>7.0380893000000002</v>
+      </c>
+      <c r="G54">
+        <v>23.838902999999998</v>
+      </c>
+    </row>
+    <row r="55" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B55">
+        <v>7.5142455000000004</v>
+      </c>
+      <c r="C55">
+        <v>21.386099999999999</v>
+      </c>
+      <c r="D55">
+        <v>8.0277560000000001</v>
+      </c>
+      <c r="E55">
+        <v>24.056376</v>
+      </c>
+      <c r="F55">
+        <v>7.5132212999999997</v>
+      </c>
+      <c r="G55">
+        <v>25.736977</v>
+      </c>
+    </row>
+    <row r="56" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B56">
+        <v>8.0024949999999997</v>
+      </c>
+      <c r="C56">
+        <v>22.161456999999999</v>
+      </c>
+      <c r="D56">
+        <v>8.5545819999999999</v>
+      </c>
+      <c r="E56">
+        <v>24.761827</v>
+      </c>
+      <c r="F56">
+        <v>8.0269619999999993</v>
+      </c>
+      <c r="G56">
+        <v>27.424795</v>
+      </c>
+    </row>
+    <row r="57" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B57">
+        <v>8.5165830000000007</v>
+      </c>
+      <c r="C57">
+        <v>22.375591</v>
+      </c>
+      <c r="D57">
+        <v>9.0300600000000006</v>
+      </c>
+      <c r="E57">
+        <v>25.186218</v>
+      </c>
+      <c r="F57">
+        <v>8.4893730000000005</v>
+      </c>
+      <c r="G57">
+        <v>28.761377</v>
+      </c>
+    </row>
+    <row r="58" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B58">
+        <v>8.9920950000000008</v>
+      </c>
+      <c r="C58">
+        <v>22.659631999999998</v>
+      </c>
+      <c r="D58">
+        <v>9.5440830000000005</v>
+      </c>
+      <c r="E58">
+        <v>25.681052999999999</v>
+      </c>
+      <c r="F58">
+        <v>9.0290189999999999</v>
+      </c>
+      <c r="G58">
+        <v>29.60727</v>
+      </c>
+    </row>
+    <row r="59" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B59">
         <v>9.5190199999999994</v>
       </c>
-      <c r="C54">
+      <c r="C59">
         <v>22.944030000000001</v>
       </c>
-      <c r="F54">
+      <c r="F59">
         <v>9.5429929999999992</v>
       </c>
-      <c r="G54">
+      <c r="G59">
         <v>30.312632000000001</v>
       </c>
     </row>
@@ -15327,7 +16335,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R36"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
+    <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
@@ -15893,8 +16901,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA57"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView topLeftCell="A25" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I42" sqref="I42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17104,8 +18112,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V131"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="P79" sqref="P79"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
micro version of duval2003faradaic parameter file
</commit_message>
<xml_diff>
--- a/2016_07_projects/reference_data.xlsx
+++ b/2016_07_projects/reference_data.xlsx
@@ -12,14 +12,14 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="16485" windowHeight="4845"/>
   </bookViews>
   <sheets>
-    <sheet name="summary" sheetId="3" r:id="rId1"/>
-    <sheet name="zhang2015control" sheetId="5" r:id="rId2"/>
-    <sheet name="duval2001bipolar" sheetId="4" r:id="rId3"/>
-    <sheet name="duval2003faradaic" sheetId="1" r:id="rId4"/>
-    <sheet name="duval2003coupling" sheetId="2" r:id="rId5"/>
+    <sheet name="notes" sheetId="6" r:id="rId1"/>
+    <sheet name="summary" sheetId="3" r:id="rId2"/>
+    <sheet name="zhang2015control" sheetId="5" r:id="rId3"/>
+    <sheet name="duval2001bipolar" sheetId="4" r:id="rId4"/>
+    <sheet name="duval2003faradaic" sheetId="1" r:id="rId5"/>
+    <sheet name="duval2003coupling" sheetId="2" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="246">
   <si>
     <t>a</t>
   </si>
@@ -583,22 +583,6 @@
     <t>done, domain composition solver, regular grid export both already set up earlier</t>
   </si>
   <si>
-    <r>
-      <t>done, domain decomposition solver, fine grid copied earlier, regular grid export, distributed sweep,</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> comsolclusterbatch</t>
-    </r>
-  </si>
-  <si>
     <t>Wbpe / m</t>
   </si>
   <si>
@@ -708,6 +692,81 @@
   </si>
   <si>
     <t>direct solver</t>
+  </si>
+  <si>
+    <t>2016_08_05_15_00_28_dses2dDirichlet_zhang2015control_iterative</t>
+  </si>
+  <si>
+    <t>GMRES</t>
+  </si>
+  <si>
+    <t>does not converge</t>
+  </si>
+  <si>
+    <t>desktop</t>
+  </si>
+  <si>
+    <t>precision 1e-6, constant newton, continuation solver</t>
+  </si>
+  <si>
+    <t>accurate on domain flux</t>
+  </si>
+  <si>
+    <t>error in parameter W</t>
+  </si>
+  <si>
+    <t>copied mesh</t>
+  </si>
+  <si>
+    <t>done, domain decomposition solver, fine grid copied earlier, regular grid export, distributed sweep, comsolclusterbatch</t>
+  </si>
+  <si>
+    <t>Error in W parameter</t>
+  </si>
+  <si>
+    <t>error in W parameter</t>
+  </si>
+  <si>
+    <t>no convergence above DeltaPHI=0.4</t>
+  </si>
+  <si>
+    <t>pde1d</t>
+  </si>
+  <si>
+    <t>Activate continuation for sweep</t>
+  </si>
+  <si>
+    <t>Before solving</t>
+  </si>
+  <si>
+    <t>dses2d</t>
+  </si>
+  <si>
+    <t>Replace X by x in flux BC</t>
+  </si>
+  <si>
+    <t>Check file name extensions in inputFiles.txt</t>
+  </si>
+  <si>
+    <t>Check if Out-Of-Core option is deactivated</t>
+  </si>
+  <si>
+    <t>Check data export operators (Global Evaluations)</t>
+  </si>
+  <si>
+    <t>general</t>
+  </si>
+  <si>
+    <t>copy Mesh</t>
+  </si>
+  <si>
+    <t>out-of-core option usually activated</t>
+  </si>
+  <si>
+    <t>Deactivate "All Derived Values"</t>
+  </si>
+  <si>
+    <t>copy UpdateInitialValue1d</t>
   </si>
 </sst>
 </file>
@@ -749,15 +808,14 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <strike/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -774,6 +832,11 @@
         <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -784,12 +847,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -802,9 +866,12 @@
     <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="3" fillId="3" borderId="0" xfId="2" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="3"/>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="0" xfId="3" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
+    <cellStyle name="Good" xfId="3" builtinId="26"/>
     <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -836,6 +903,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1541,6 +1609,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -9441,6 +9510,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -14505,10 +14575,85 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L43"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>241</v>
+      </c>
+      <c r="B2" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>233</v>
+      </c>
+      <c r="B4" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>236</v>
+      </c>
+      <c r="B7" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>240</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L48"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14548,7 +14693,7 @@
         <v>181</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I2" t="s">
         <v>172</v>
@@ -14642,417 +14787,467 @@
         <v>167</v>
       </c>
       <c r="J8" s="9" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="K8" s="6" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D9" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D9" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="E9" t="s">
-        <v>215</v>
-      </c>
-      <c r="F9" s="8">
+      <c r="E9" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="F9" s="9">
         <v>42592</v>
       </c>
-      <c r="H9" s="8" t="s">
-        <v>211</v>
-      </c>
-      <c r="J9" s="8"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="J10" s="8"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="J9" s="9" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D10" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="F10" s="10">
+        <v>42594</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="I10" s="7" t="s">
+        <v>228</v>
+      </c>
+      <c r="J10" s="7" t="s">
+        <v>232</v>
+      </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
+      <c r="F11"/>
+      <c r="G11"/>
+      <c r="H11"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
         <v>135</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D12" t="s">
         <v>138</v>
       </c>
-      <c r="F11" s="8">
+      <c r="F12" s="8">
         <v>42566</v>
       </c>
-      <c r="I11" t="s">
+      <c r="I12" t="s">
         <v>139</v>
       </c>
-      <c r="J11" t="s">
+      <c r="J12" t="s">
         <v>140</v>
       </c>
-      <c r="K11" t="s">
+      <c r="K12" t="s">
         <v>150</v>
       </c>
-      <c r="L11" t="s">
+      <c r="L12" t="s">
         <v>148</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D12" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="6" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="13" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D13" s="6" t="s">
         <v>151</v>
       </c>
-      <c r="E13" s="6" t="s">
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="6" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D14" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="F14" s="9">
+        <v>42579</v>
+      </c>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="I14" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="J14" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="K14" s="6" t="s">
         <v>218</v>
       </c>
-      <c r="F13" s="9">
-        <v>42579</v>
-      </c>
-      <c r="G13" s="9"/>
-      <c r="H13" s="9" t="s">
-        <v>211</v>
-      </c>
-      <c r="I13" s="6" t="s">
+    </row>
+    <row r="15" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D15" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="F15" s="9">
+        <v>42592</v>
+      </c>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="I15" s="6" t="s">
         <v>167</v>
       </c>
-      <c r="J13" s="6" t="s">
+      <c r="J15" s="9" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D16" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="F16" s="10">
+        <v>42594</v>
+      </c>
+      <c r="G16" s="10"/>
+      <c r="H16" s="10" t="s">
         <v>210</v>
       </c>
-      <c r="K13" s="6" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D14" t="s">
-        <v>151</v>
-      </c>
-      <c r="E14" t="s">
-        <v>217</v>
-      </c>
-      <c r="F14" s="8">
-        <v>42592</v>
-      </c>
-      <c r="H14" s="8" t="s">
-        <v>211</v>
-      </c>
-      <c r="I14" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="6" t="s">
+      <c r="I16" s="7" t="s">
+        <v>228</v>
+      </c>
+      <c r="J16" s="7" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="D18" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="F16" s="9">
+      <c r="F18" s="9">
         <v>42566</v>
       </c>
-      <c r="G16" s="9"/>
-      <c r="H16" s="9"/>
-      <c r="I16" s="6" t="s">
-        <v>142</v>
-      </c>
-      <c r="J16" s="6" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="17" spans="2:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D17" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="F17" s="10">
-        <v>42578</v>
-      </c>
-      <c r="G17" s="10"/>
-      <c r="H17" s="10"/>
-      <c r="I17" s="7" t="s">
-        <v>167</v>
-      </c>
-      <c r="J17" s="7" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="18" spans="2:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D18" s="6" t="s">
-        <v>152</v>
-      </c>
-      <c r="F18" s="9"/>
       <c r="G18" s="9"/>
       <c r="H18" s="9"/>
       <c r="I18" s="6" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="19" spans="2:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D19" s="6" t="s">
-        <v>152</v>
-      </c>
-      <c r="F19" s="9">
+      <c r="J18" s="6" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="19" spans="2:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D19" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="F19" s="10">
         <v>42578</v>
       </c>
-      <c r="G19" s="9"/>
-      <c r="H19" s="9"/>
-      <c r="I19" s="6" t="s">
+      <c r="G19" s="10"/>
+      <c r="H19" s="10"/>
+      <c r="I19" s="7" t="s">
         <v>167</v>
       </c>
-      <c r="J19" s="6" t="s">
-        <v>169</v>
+      <c r="J19" s="7" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="20" spans="2:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D20" s="6" t="s">
         <v>152</v>
       </c>
-      <c r="E20" s="6" t="s">
-        <v>216</v>
-      </c>
-      <c r="F20" s="9">
-        <v>42579</v>
-      </c>
-      <c r="G20" s="9">
-        <v>42583</v>
-      </c>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
       <c r="H20" s="9"/>
       <c r="I20" s="6" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="21" spans="2:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D21" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="F21" s="9">
+        <v>42578</v>
+      </c>
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="6" t="s">
         <v>167</v>
       </c>
-      <c r="J20" s="6" t="s">
+      <c r="J21" s="6" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="22" spans="2:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D22" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="F22" s="9">
+        <v>42579</v>
+      </c>
+      <c r="G22" s="9">
+        <v>42583</v>
+      </c>
+      <c r="H22" s="9"/>
+      <c r="I22" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="J22" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="K22" s="6" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="23" spans="2:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D23" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="F23" s="9">
+        <v>42592</v>
+      </c>
+      <c r="G23" s="9"/>
+      <c r="H23" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="I23" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="J23" s="6" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="24" spans="2:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D24" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="F24" s="13">
+        <v>42594</v>
+      </c>
+      <c r="G24" s="13"/>
+      <c r="H24" s="13" t="s">
+        <v>210</v>
+      </c>
+      <c r="I24" s="12" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>146</v>
+      </c>
+      <c r="D26" t="s">
+        <v>145</v>
+      </c>
+      <c r="F26" s="8">
+        <v>42568</v>
+      </c>
+      <c r="I26" t="s">
+        <v>147</v>
+      </c>
+      <c r="J26" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="27" spans="2:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D27" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="F27" s="9">
+        <v>42574</v>
+      </c>
+      <c r="G27" s="9"/>
+      <c r="H27" s="9"/>
+      <c r="I27" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="J27" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="K27" s="6" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="28" spans="2:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D28" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>229</v>
+      </c>
+      <c r="F28" s="9">
+        <v>42579</v>
+      </c>
+      <c r="G28" s="9"/>
+      <c r="H28" s="9"/>
+      <c r="I28" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="J28" s="6" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="29" spans="2:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D29" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="F29" s="9"/>
+      <c r="G29" s="9"/>
+      <c r="H29" s="9"/>
+      <c r="I29" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="J29" s="6" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="30" spans="2:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D30" s="12" t="s">
+        <v>153</v>
+      </c>
+      <c r="F30" s="13">
+        <v>42594</v>
+      </c>
+      <c r="I30" s="12" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="33" spans="2:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="F33" s="9">
+        <v>42575</v>
+      </c>
+      <c r="G33" s="9"/>
+      <c r="H33" s="9"/>
+      <c r="I33" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="J33" s="6" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="34" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C34" t="s">
+        <v>96</v>
+      </c>
+      <c r="D34" t="s">
+        <v>157</v>
+      </c>
+      <c r="F34" s="8">
+        <v>42578</v>
+      </c>
+      <c r="G34" s="8">
+        <v>42579</v>
+      </c>
+      <c r="I34" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="35" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C35" t="s">
+        <v>96</v>
+      </c>
+      <c r="D35" t="s">
+        <v>182</v>
+      </c>
+      <c r="E35" t="s">
+        <v>183</v>
+      </c>
+      <c r="F35" s="8">
+        <v>42579</v>
+      </c>
+      <c r="I35" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="40" spans="2:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="6" t="s">
+        <v>198</v>
+      </c>
+      <c r="D40" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="F40" s="9">
+        <v>42583</v>
+      </c>
+      <c r="G40" s="9">
+        <v>42583</v>
+      </c>
+      <c r="H40" s="9"/>
+      <c r="J40" s="6" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="41" spans="2:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D41" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="F41" s="9">
+        <v>42583</v>
+      </c>
+      <c r="G41" s="9">
+        <v>42584</v>
+      </c>
+      <c r="H41" s="9"/>
+      <c r="J41" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="K41" s="6" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="42" spans="2:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D42" s="6" t="s">
         <v>204</v>
       </c>
-      <c r="K20" s="6" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="D21" t="s">
-        <v>152</v>
-      </c>
-      <c r="E21" t="s">
-        <v>215</v>
-      </c>
-      <c r="F21" s="8">
-        <v>42592</v>
-      </c>
-      <c r="H21" s="8" t="s">
-        <v>211</v>
-      </c>
-      <c r="I21" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
-        <v>146</v>
-      </c>
-      <c r="D23" t="s">
-        <v>145</v>
-      </c>
-      <c r="F23" s="8">
-        <v>42568</v>
-      </c>
-      <c r="I23" t="s">
-        <v>147</v>
-      </c>
-      <c r="J23" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="24" spans="2:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D24" s="6" t="s">
-        <v>153</v>
-      </c>
-      <c r="F24" s="9">
-        <v>42574</v>
-      </c>
-      <c r="G24" s="9"/>
-      <c r="H24" s="9"/>
-      <c r="I24" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="J24" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="K24" s="6" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="D25" t="s">
-        <v>153</v>
-      </c>
-      <c r="E25" t="s">
-        <v>184</v>
-      </c>
-      <c r="F25" s="8">
-        <v>42579</v>
-      </c>
-      <c r="I25" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="D26" t="s">
-        <v>220</v>
-      </c>
-      <c r="E26" t="s">
-        <v>221</v>
-      </c>
-      <c r="I26" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="30" spans="2:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="C30" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="D30" s="6" t="s">
-        <v>157</v>
-      </c>
-      <c r="F30" s="9">
-        <v>42575</v>
-      </c>
-      <c r="G30" s="9"/>
-      <c r="H30" s="9"/>
-      <c r="I30" s="6" t="s">
-        <v>158</v>
-      </c>
-      <c r="J30" s="6" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C31" t="s">
-        <v>96</v>
-      </c>
-      <c r="D31" t="s">
-        <v>157</v>
-      </c>
-      <c r="F31" s="8">
-        <v>42578</v>
-      </c>
-      <c r="G31" s="8">
-        <v>42579</v>
-      </c>
-      <c r="I31" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C32" t="s">
-        <v>96</v>
-      </c>
-      <c r="D32" t="s">
-        <v>182</v>
-      </c>
-      <c r="E32" t="s">
-        <v>183</v>
-      </c>
-      <c r="F32" s="8">
-        <v>42579</v>
-      </c>
-      <c r="I32" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="37" spans="2:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="6" t="s">
-        <v>199</v>
-      </c>
-      <c r="D37" s="6" t="s">
-        <v>200</v>
-      </c>
-      <c r="F37" s="9">
-        <v>42583</v>
-      </c>
-      <c r="G37" s="9">
-        <v>42583</v>
-      </c>
-      <c r="H37" s="9"/>
-      <c r="J37" s="6" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="38" spans="2:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D38" s="6" t="s">
-        <v>202</v>
-      </c>
-      <c r="F38" s="9">
-        <v>42583</v>
-      </c>
-      <c r="G38" s="9">
-        <v>42584</v>
-      </c>
-      <c r="H38" s="9"/>
-      <c r="J38" s="6" t="s">
-        <v>203</v>
-      </c>
-      <c r="K38" s="6" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="39" spans="2:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D39" s="6" t="s">
+      <c r="E42" s="6" t="s">
         <v>205</v>
       </c>
-      <c r="E39" s="6" t="s">
+      <c r="F42" s="9">
+        <v>42587</v>
+      </c>
+      <c r="G42" s="9">
+        <v>42587</v>
+      </c>
+      <c r="H42" s="9"/>
+      <c r="K42" s="6" t="s">
         <v>206</v>
-      </c>
-      <c r="F39" s="9">
-        <v>42587</v>
-      </c>
-      <c r="G39" s="9">
-        <v>42587</v>
-      </c>
-      <c r="H39" s="9"/>
-      <c r="K39" s="6" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="40" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="D40" t="s">
-        <v>202</v>
-      </c>
-      <c r="F40" s="8">
-        <v>42587</v>
-      </c>
-      <c r="G40" s="8">
-        <v>42587</v>
-      </c>
-    </row>
-    <row r="41" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="D41" t="s">
-        <v>205</v>
-      </c>
-      <c r="F41" s="8">
-        <v>42587</v>
-      </c>
-      <c r="G41" s="8">
-        <v>42587</v>
-      </c>
-    </row>
-    <row r="42" spans="2:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D42" s="7" t="s">
-        <v>208</v>
-      </c>
-      <c r="F42" s="10">
-        <v>42588</v>
-      </c>
-      <c r="G42" s="10"/>
-      <c r="H42" s="10"/>
-      <c r="J42" s="7" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="43" spans="2:11" x14ac:dyDescent="0.25">
       <c r="D43" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="F43" s="8">
         <v>42587</v>
@@ -15060,8 +15255,77 @@
       <c r="G43" s="8">
         <v>42587</v>
       </c>
-      <c r="J43" t="s">
-        <v>214</v>
+    </row>
+    <row r="44" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="D44" t="s">
+        <v>204</v>
+      </c>
+      <c r="F44" s="8">
+        <v>42587</v>
+      </c>
+      <c r="G44" s="8">
+        <v>42587</v>
+      </c>
+    </row>
+    <row r="45" spans="2:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D45" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="F45" s="10">
+        <v>42588</v>
+      </c>
+      <c r="G45" s="10"/>
+      <c r="H45" s="10"/>
+      <c r="J45" s="7" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="46" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="D46" t="s">
+        <v>207</v>
+      </c>
+      <c r="F46" s="8">
+        <v>42587</v>
+      </c>
+      <c r="G46" s="8">
+        <v>42587</v>
+      </c>
+      <c r="J46" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="47" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="D47" t="s">
+        <v>221</v>
+      </c>
+      <c r="E47" t="s">
+        <v>222</v>
+      </c>
+      <c r="F47" s="8">
+        <v>42593</v>
+      </c>
+      <c r="J47" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="48" spans="2:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D48" s="12" t="s">
+        <v>207</v>
+      </c>
+      <c r="E48" s="12" t="s">
+        <v>225</v>
+      </c>
+      <c r="F48" s="13">
+        <v>42594</v>
+      </c>
+      <c r="G48" s="13">
+        <v>42594</v>
+      </c>
+      <c r="H48" s="13" t="s">
+        <v>224</v>
+      </c>
+      <c r="J48" s="12" t="s">
+        <v>226</v>
       </c>
     </row>
   </sheetData>
@@ -15070,12 +15334,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA59"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q28" sqref="Q28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15088,7 +15352,7 @@
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B1" s="1">
         <f>B3+2*B2</f>
@@ -15121,7 +15385,7 @@
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B2" s="1">
         <v>5.0000000000000001E-4</v>
@@ -15172,7 +15436,7 @@
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B3" s="1">
         <v>0.01</v>
@@ -15238,7 +15502,7 @@
         <v>1</v>
       </c>
       <c r="P4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="Q4" s="11">
         <v>6.3899999999999996E-10</v>
@@ -15278,7 +15542,7 @@
         <v>1</v>
       </c>
       <c r="P5" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="Q5" s="11">
         <v>1.3339999999999999E-9</v>
@@ -15311,7 +15575,7 @@
     <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="O6" s="1"/>
       <c r="P6" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="Q6" s="11">
         <v>1.792E-9</v>
@@ -15355,14 +15619,14 @@
         <v>164</v>
       </c>
       <c r="T8" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="U8" s="1">
         <f>SUM(U2:U6)</f>
         <v>0.1185099978503988</v>
       </c>
       <c r="V8" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="W8" s="1"/>
       <c r="X8" s="1"/>
@@ -15388,7 +15652,7 @@
         <v>0.4</v>
       </c>
       <c r="V9" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.25">
@@ -15810,7 +16074,7 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B32">
         <f>B30-B12</f>
@@ -15842,12 +16106,12 @@
         <v>0.56413082986480123</v>
       </c>
       <c r="H33" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B34" s="1">
         <f>$U$8*B$33</f>
@@ -15866,7 +16130,7 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B35" s="1">
         <f>B$10/B$34</f>
@@ -15883,7 +16147,7 @@
         <v>5.9830849123996927E-3</v>
       </c>
       <c r="I35" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
@@ -16331,12 +16595,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R36"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="R22" sqref="R22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16897,12 +17161,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA57"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I42" sqref="I42"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18108,12 +18372,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V131"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A49" sqref="A49"/>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="J64" sqref="J64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Made some parameter file zhang20015inert.m without reactions and did some necessary changes in scripts
</commit_message>
<xml_diff>
--- a/2016_07_projects/reference_data.xlsx
+++ b/2016_07_projects/reference_data.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="258">
   <si>
     <t>a</t>
   </si>
@@ -767,6 +767,42 @@
   </si>
   <si>
     <t>copy UpdateInitialValue1d</t>
+  </si>
+  <si>
+    <t>tcd2dZNC</t>
+  </si>
+  <si>
+    <t>adjust data 2 export mesh nodes</t>
+  </si>
+  <si>
+    <t>Log: Study &gt; Solver Configuration &gt; Solution &gt; Stationary Solver &gt; Log &gt; Keep warnings in stored log</t>
+  </si>
+  <si>
+    <t>Log: Study &gt; Solver Configuration &gt; Solution &gt; Stationary Solver &gt; Advanced &gt; Solver log: Detailed</t>
+  </si>
+  <si>
+    <t>Manually add intBPE operator</t>
+  </si>
+  <si>
+    <t>Adjust PHI_bpe Potential</t>
+  </si>
+  <si>
+    <t>corrected</t>
+  </si>
+  <si>
+    <t>MATLAB code</t>
+  </si>
+  <si>
+    <t>tcd2d</t>
+  </si>
+  <si>
+    <t>adjust export mesh</t>
+  </si>
+  <si>
+    <t>switch to constant Newton</t>
+  </si>
+  <si>
+    <t>corrected for tcd</t>
   </si>
 </sst>
 </file>
@@ -903,7 +939,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1609,7 +1644,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2471,7 +2505,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3438,7 +3471,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3520,7 +3552,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4381,7 +4412,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5061,7 +5091,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6614,7 +6643,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7831,7 +7859,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -8573,7 +8600,6 @@
           </c:spPr>
         </c:majorGridlines>
         <c:title>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -8666,7 +8692,6 @@
           </c:spPr>
         </c:majorGridlines>
         <c:title>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -8747,7 +8772,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -9510,7 +9534,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -14575,20 +14598,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>235</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>241</v>
       </c>
@@ -14596,50 +14622,100 @@
         <v>242</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="E3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>254</v>
+      </c>
+      <c r="B6" t="s">
+        <v>255</v>
+      </c>
+      <c r="E6" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>246</v>
+      </c>
+      <c r="B8" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>233</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B9" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>236</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B12" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
         <v>240</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>250</v>
+      </c>
+      <c r="E16" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>251</v>
       </c>
     </row>
   </sheetData>
@@ -14652,13 +14728,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L48"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="19.5703125" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" customWidth="1"/>
     <col min="3" max="3" width="7.7109375" customWidth="1"/>
     <col min="4" max="5" width="77" customWidth="1"/>
     <col min="6" max="6" width="10.7109375" style="8" bestFit="1" customWidth="1"/>
@@ -15339,7 +15415,7 @@
   <dimension ref="A1:AA59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Q28" sqref="Q28"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16599,8 +16675,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R36"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="R22" sqref="R22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
More isotherm plots in 2016_10
</commit_message>
<xml_diff>
--- a/2016_07_projects/reference_data.xlsx
+++ b/2016_07_projects/reference_data.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="292">
   <si>
     <t>a</t>
   </si>
@@ -907,6 +907,9 @@
   <si>
     <t>I / A m-^2</t>
   </si>
+  <si>
+    <t>m / g m^-2</t>
+  </si>
 </sst>
 </file>
 
@@ -4392,7 +4395,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -8841,6 +8843,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -22766,16 +22769,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>59</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -23646,7 +23649,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V131"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" workbookViewId="0">
+    <sheetView topLeftCell="A43" workbookViewId="0">
       <selection activeCell="J64" sqref="J64"/>
     </sheetView>
   </sheetViews>
@@ -27246,12 +27249,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12:N30"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="O56" sqref="O56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="9" max="10" width="12" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="11.5703125" customWidth="1"/>
     <col min="17" max="17" width="10" style="11" customWidth="1"/>
     <col min="19" max="19" width="12.28515625" customWidth="1"/>
@@ -28907,6 +28911,15 @@
       <c r="F39">
         <v>0.4</v>
       </c>
+      <c r="I39">
+        <v>0.1</v>
+      </c>
+      <c r="K39">
+        <v>0.2</v>
+      </c>
+      <c r="M39">
+        <v>0.4</v>
+      </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
@@ -28927,6 +28940,24 @@
       <c r="G40" t="s">
         <v>166</v>
       </c>
+      <c r="I40" t="s">
+        <v>270</v>
+      </c>
+      <c r="J40" t="s">
+        <v>291</v>
+      </c>
+      <c r="K40" t="s">
+        <v>270</v>
+      </c>
+      <c r="L40" t="s">
+        <v>291</v>
+      </c>
+      <c r="M40" t="s">
+        <v>270</v>
+      </c>
+      <c r="N40" t="s">
+        <v>291</v>
+      </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B41">
@@ -28947,6 +28978,30 @@
       <c r="G41">
         <v>2.3893925999999999</v>
       </c>
+      <c r="I41">
+        <f>(B41-5)/1000</f>
+        <v>-4.4867046000000004E-3</v>
+      </c>
+      <c r="J41">
+        <f>C41*0.000000000001*(100^2)</f>
+        <v>3.5825552999999999E-8</v>
+      </c>
+      <c r="K41">
+        <f>(D41-5)/1000</f>
+        <v>-4.4993763600000005E-3</v>
+      </c>
+      <c r="L41">
+        <f>E41*0.000000000001*(100^2)</f>
+        <v>2.8105354E-8</v>
+      </c>
+      <c r="M41">
+        <f>(F41-5)/1000</f>
+        <v>-4.5121306499999996E-3</v>
+      </c>
+      <c r="N41">
+        <f>G41*0.000000000001*(100^2)</f>
+        <v>2.3893925999999995E-8</v>
+      </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B42">
@@ -28967,6 +29022,30 @@
       <c r="G42">
         <v>2.6737022000000001</v>
       </c>
+      <c r="I42">
+        <f t="shared" ref="I42:I58" si="21">(B42-5)/1000</f>
+        <v>-3.9855191999999999E-3</v>
+      </c>
+      <c r="J42">
+        <f t="shared" ref="J42:J59" si="22">C42*0.000000000001*(100^2)</f>
+        <v>4.0071260000000005E-8</v>
+      </c>
+      <c r="K42">
+        <f t="shared" ref="K42:K58" si="23">(D42-5)/1000</f>
+        <v>-3.9596470000000002E-3</v>
+      </c>
+      <c r="L42">
+        <f t="shared" ref="L42:L58" si="24">E42*0.000000000001*(100^2)</f>
+        <v>3.3055518E-8</v>
+      </c>
+      <c r="M42">
+        <f t="shared" ref="M42:M59" si="25">(F42-5)/1000</f>
+        <v>-3.9980587999999999E-3</v>
+      </c>
+      <c r="N42">
+        <f t="shared" ref="N42:N59" si="26">G42*0.000000000001*(100^2)</f>
+        <v>2.6737022000000004E-8</v>
+      </c>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B43">
@@ -28987,6 +29066,30 @@
       <c r="G43">
         <v>3.0280971999999999</v>
       </c>
+      <c r="I43">
+        <f t="shared" si="21"/>
+        <v>-3.471596E-3</v>
+      </c>
+      <c r="J43">
+        <f t="shared" si="22"/>
+        <v>4.9230146000000005E-8</v>
+      </c>
+      <c r="K43">
+        <f t="shared" si="23"/>
+        <v>-3.4970550000000002E-3</v>
+      </c>
+      <c r="L43">
+        <f t="shared" si="24"/>
+        <v>3.8702025000000003E-8</v>
+      </c>
+      <c r="M43">
+        <f t="shared" si="25"/>
+        <v>-3.4968567999999998E-3</v>
+      </c>
+      <c r="N43">
+        <f t="shared" si="26"/>
+        <v>3.0280972000000003E-8</v>
+      </c>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B44">
@@ -29007,6 +29110,30 @@
       <c r="G44">
         <v>3.4524872000000002</v>
       </c>
+      <c r="I44">
+        <f t="shared" si="21"/>
+        <v>-2.9833962999999998E-3</v>
+      </c>
+      <c r="J44">
+        <f t="shared" si="22"/>
+        <v>5.9088983999999995E-8</v>
+      </c>
+      <c r="K44">
+        <f t="shared" si="23"/>
+        <v>-2.9959028000000002E-3</v>
+      </c>
+      <c r="L44">
+        <f t="shared" si="24"/>
+        <v>4.4351240000000002E-8</v>
+      </c>
+      <c r="M44">
+        <f t="shared" si="25"/>
+        <v>-3.0213783999999996E-3</v>
+      </c>
+      <c r="N44">
+        <f t="shared" si="26"/>
+        <v>3.4524871999999999E-8</v>
+      </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B45">
@@ -29027,6 +29154,30 @@
       <c r="G45">
         <v>4.3683759999999996</v>
       </c>
+      <c r="I45">
+        <f t="shared" si="21"/>
+        <v>-2.4824090000000001E-3</v>
+      </c>
+      <c r="J45">
+        <f t="shared" si="22"/>
+        <v>7.1755739999999994E-8</v>
+      </c>
+      <c r="K45">
+        <f t="shared" si="23"/>
+        <v>-2.4948660999999997E-3</v>
+      </c>
+      <c r="L45">
+        <f t="shared" si="24"/>
+        <v>5.4912733999999991E-8</v>
+      </c>
+      <c r="M45">
+        <f t="shared" si="25"/>
+        <v>-2.507455E-3</v>
+      </c>
+      <c r="N45">
+        <f t="shared" si="26"/>
+        <v>4.3683759999999999E-8</v>
+      </c>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B46">
@@ -29047,6 +29198,30 @@
       <c r="G46">
         <v>5.2139990000000003</v>
       </c>
+      <c r="I46">
+        <f t="shared" si="21"/>
+        <v>-2.0072445999999998E-3</v>
+      </c>
+      <c r="J46">
+        <f t="shared" si="22"/>
+        <v>8.9332970000000007E-8</v>
+      </c>
+      <c r="K46">
+        <f t="shared" si="23"/>
+        <v>-1.9810914999999997E-3</v>
+      </c>
+      <c r="L46">
+        <f t="shared" si="24"/>
+        <v>7.0387405999999997E-8</v>
+      </c>
+      <c r="M46">
+        <f t="shared" si="25"/>
+        <v>-2.0063689E-3</v>
+      </c>
+      <c r="N46">
+        <f t="shared" si="26"/>
+        <v>5.2139990000000006E-8</v>
+      </c>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B47">
@@ -29067,6 +29242,30 @@
       <c r="G47">
         <v>6.7613763999999996</v>
       </c>
+      <c r="I47">
+        <f t="shared" si="21"/>
+        <v>-1.480699E-3</v>
+      </c>
+      <c r="J47">
+        <f t="shared" si="22"/>
+        <v>1.0831733E-7</v>
+      </c>
+      <c r="K47">
+        <f t="shared" si="23"/>
+        <v>-1.4931230000000003E-3</v>
+      </c>
+      <c r="L47">
+        <f t="shared" si="24"/>
+        <v>9.0070809999999999E-8</v>
+      </c>
+      <c r="M47">
+        <f t="shared" si="25"/>
+        <v>-1.5054479000000001E-3</v>
+      </c>
+      <c r="N47">
+        <f t="shared" si="26"/>
+        <v>6.761376399999999E-8</v>
+      </c>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B48">
@@ -29087,8 +29286,32 @@
       <c r="G48">
         <v>8.8003429999999998</v>
       </c>
-    </row>
-    <row r="49" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I48">
+        <f t="shared" si="21"/>
+        <v>-9.6695759999999972E-4</v>
+      </c>
+      <c r="J48">
+        <f t="shared" si="22"/>
+        <v>1.2519551E-7</v>
+      </c>
+      <c r="K48">
+        <f t="shared" si="23"/>
+        <v>-9.9236729999999974E-4</v>
+      </c>
+      <c r="L48">
+        <f t="shared" si="24"/>
+        <v>1.1256212E-7</v>
+      </c>
+      <c r="M48">
+        <f t="shared" si="25"/>
+        <v>-9.5322849999999982E-4</v>
+      </c>
+      <c r="N48">
+        <f t="shared" si="26"/>
+        <v>8.8003429999999995E-8</v>
+      </c>
+    </row>
+    <row r="49" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B49">
         <v>4.520994</v>
       </c>
@@ -29107,8 +29330,32 @@
       <c r="G49">
         <v>11.330266999999999</v>
       </c>
-    </row>
-    <row r="50" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I49">
+        <f t="shared" si="21"/>
+        <v>-4.7900600000000003E-4</v>
+      </c>
+      <c r="J49">
+        <f t="shared" si="22"/>
+        <v>1.4558066E-7</v>
+      </c>
+      <c r="K49">
+        <f t="shared" si="23"/>
+        <v>-4.9169399999999988E-4</v>
+      </c>
+      <c r="L49">
+        <f t="shared" si="24"/>
+        <v>1.3856220999999999E-7</v>
+      </c>
+      <c r="M49">
+        <f t="shared" si="25"/>
+        <v>-4.3968529999999982E-4</v>
+      </c>
+      <c r="N49">
+        <f t="shared" si="26"/>
+        <v>1.1330266999999999E-7</v>
+      </c>
+    </row>
+    <row r="50" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B50">
         <v>5.0474569999999996</v>
       </c>
@@ -29127,8 +29374,32 @@
       <c r="G50">
         <v>13.789564</v>
       </c>
-    </row>
-    <row r="51" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I50">
+        <f t="shared" si="21"/>
+        <v>4.7456999999999637E-5</v>
+      </c>
+      <c r="J50">
+        <f t="shared" si="22"/>
+        <v>1.6807379000000001E-7</v>
+      </c>
+      <c r="K50">
+        <f t="shared" si="23"/>
+        <v>2.1866000000000163E-5</v>
+      </c>
+      <c r="L50">
+        <f t="shared" si="24"/>
+        <v>1.6315969999999998E-7</v>
+      </c>
+      <c r="M50">
+        <f t="shared" si="25"/>
+        <v>9.6069999999999217E-6</v>
+      </c>
+      <c r="N50">
+        <f t="shared" si="26"/>
+        <v>1.3789564E-7</v>
+      </c>
+    </row>
+    <row r="51" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B51">
         <v>5.5354752999999999</v>
       </c>
@@ -29147,8 +29418,32 @@
       <c r="G51">
         <v>16.319396999999999</v>
       </c>
-    </row>
-    <row r="52" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I51">
+        <f t="shared" si="21"/>
+        <v>5.3547529999999988E-4</v>
+      </c>
+      <c r="J51">
+        <f t="shared" si="22"/>
+        <v>1.8565190999999999E-7</v>
+      </c>
+      <c r="K51">
+        <f t="shared" si="23"/>
+        <v>5.2267099999999983E-4</v>
+      </c>
+      <c r="L51">
+        <f t="shared" si="24"/>
+        <v>1.8354576000000002E-7</v>
+      </c>
+      <c r="M51">
+        <f t="shared" si="25"/>
+        <v>5.1029699999999951E-4</v>
+      </c>
+      <c r="N51">
+        <f t="shared" si="26"/>
+        <v>1.6319397E-7</v>
+      </c>
+    </row>
+    <row r="52" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B52">
         <v>6.0236749999999999</v>
       </c>
@@ -29167,8 +29462,32 @@
       <c r="G52">
         <v>18.779057000000002</v>
       </c>
-    </row>
-    <row r="53" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I52">
+        <f t="shared" si="21"/>
+        <v>1.0236749999999999E-3</v>
+      </c>
+      <c r="J52">
+        <f t="shared" si="22"/>
+        <v>1.9551075E-7</v>
+      </c>
+      <c r="K52">
+        <f t="shared" si="23"/>
+        <v>9.9788500000000022E-4</v>
+      </c>
+      <c r="L52">
+        <f t="shared" si="24"/>
+        <v>1.9901772000000003E-7</v>
+      </c>
+      <c r="M52">
+        <f t="shared" si="25"/>
+        <v>1.0110029999999997E-3</v>
+      </c>
+      <c r="N52">
+        <f t="shared" si="26"/>
+        <v>1.8779056999999999E-7</v>
+      </c>
+    </row>
+    <row r="53" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B53">
         <v>6.4990873000000002</v>
       </c>
@@ -29187,8 +29506,32 @@
       <c r="G53">
         <v>21.308800000000002</v>
       </c>
-    </row>
-    <row r="54" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I53">
+        <f t="shared" si="21"/>
+        <v>1.4990873000000002E-3</v>
+      </c>
+      <c r="J53">
+        <f t="shared" si="22"/>
+        <v>2.0256166E-7</v>
+      </c>
+      <c r="K53">
+        <f t="shared" si="23"/>
+        <v>2.0127625000000001E-3</v>
+      </c>
+      <c r="L53">
+        <f t="shared" si="24"/>
+        <v>2.2224688000000001E-7</v>
+      </c>
+      <c r="M53">
+        <f t="shared" si="25"/>
+        <v>1.4988393999999996E-3</v>
+      </c>
+      <c r="N53">
+        <f t="shared" si="26"/>
+        <v>2.1308800000000001E-7</v>
+      </c>
+    </row>
+    <row r="54" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B54">
         <v>6.9873529999999997</v>
       </c>
@@ -29207,8 +29550,32 @@
       <c r="G54">
         <v>23.838902999999998</v>
       </c>
-    </row>
-    <row r="55" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I54">
+        <f t="shared" si="21"/>
+        <v>1.9873529999999999E-3</v>
+      </c>
+      <c r="J54">
+        <f t="shared" si="22"/>
+        <v>2.0961349999999997E-7</v>
+      </c>
+      <c r="K54">
+        <f t="shared" si="23"/>
+        <v>2.5523924999999999E-3</v>
+      </c>
+      <c r="L54">
+        <f t="shared" si="24"/>
+        <v>2.3140757000000001E-7</v>
+      </c>
+      <c r="M54">
+        <f t="shared" si="25"/>
+        <v>2.0380893000000004E-3</v>
+      </c>
+      <c r="N54">
+        <f t="shared" si="26"/>
+        <v>2.3838902999999998E-7</v>
+      </c>
+    </row>
+    <row r="55" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B55">
         <v>7.5142455000000004</v>
       </c>
@@ -29227,8 +29594,32 @@
       <c r="G55">
         <v>25.736977</v>
       </c>
-    </row>
-    <row r="56" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I55">
+        <f t="shared" si="21"/>
+        <v>2.5142455000000002E-3</v>
+      </c>
+      <c r="J55">
+        <f t="shared" si="22"/>
+        <v>2.1386099999999999E-7</v>
+      </c>
+      <c r="K55">
+        <f t="shared" si="23"/>
+        <v>3.0277559999999999E-3</v>
+      </c>
+      <c r="L55">
+        <f t="shared" si="24"/>
+        <v>2.4056376000000001E-7</v>
+      </c>
+      <c r="M55">
+        <f t="shared" si="25"/>
+        <v>2.5132212999999996E-3</v>
+      </c>
+      <c r="N55">
+        <f t="shared" si="26"/>
+        <v>2.5736976999999999E-7</v>
+      </c>
+    </row>
+    <row r="56" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B56">
         <v>8.0024949999999997</v>
       </c>
@@ -29247,8 +29638,32 @@
       <c r="G56">
         <v>27.424795</v>
       </c>
-    </row>
-    <row r="57" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I56">
+        <f t="shared" si="21"/>
+        <v>3.0024949999999996E-3</v>
+      </c>
+      <c r="J56">
+        <f t="shared" si="22"/>
+        <v>2.2161456999999999E-7</v>
+      </c>
+      <c r="K56">
+        <f t="shared" si="23"/>
+        <v>3.5545819999999997E-3</v>
+      </c>
+      <c r="L56">
+        <f t="shared" si="24"/>
+        <v>2.4761826999999996E-7</v>
+      </c>
+      <c r="M56">
+        <f t="shared" si="25"/>
+        <v>3.0269619999999994E-3</v>
+      </c>
+      <c r="N56">
+        <f t="shared" si="26"/>
+        <v>2.7424794999999999E-7</v>
+      </c>
+    </row>
+    <row r="57" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B57">
         <v>8.5165830000000007</v>
       </c>
@@ -29267,8 +29682,32 @@
       <c r="G57">
         <v>28.761377</v>
       </c>
-    </row>
-    <row r="58" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I57">
+        <f t="shared" si="21"/>
+        <v>3.5165830000000006E-3</v>
+      </c>
+      <c r="J57">
+        <f t="shared" si="22"/>
+        <v>2.2375591E-7</v>
+      </c>
+      <c r="K57">
+        <f t="shared" si="23"/>
+        <v>4.0300600000000002E-3</v>
+      </c>
+      <c r="L57">
+        <f t="shared" si="24"/>
+        <v>2.5186218E-7</v>
+      </c>
+      <c r="M57">
+        <f t="shared" si="25"/>
+        <v>3.4893730000000005E-3</v>
+      </c>
+      <c r="N57">
+        <f t="shared" si="26"/>
+        <v>2.8761376999999998E-7</v>
+      </c>
+    </row>
+    <row r="58" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B58">
         <v>8.9920950000000008</v>
       </c>
@@ -29287,8 +29726,32 @@
       <c r="G58">
         <v>29.60727</v>
       </c>
-    </row>
-    <row r="59" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I58">
+        <f t="shared" si="21"/>
+        <v>3.9920950000000011E-3</v>
+      </c>
+      <c r="J58">
+        <f t="shared" si="22"/>
+        <v>2.2659631999999997E-7</v>
+      </c>
+      <c r="K58">
+        <f t="shared" si="23"/>
+        <v>4.5440830000000008E-3</v>
+      </c>
+      <c r="L58">
+        <f t="shared" si="24"/>
+        <v>2.5681053E-7</v>
+      </c>
+      <c r="M58">
+        <f t="shared" si="25"/>
+        <v>4.029019E-3</v>
+      </c>
+      <c r="N58">
+        <f t="shared" si="26"/>
+        <v>2.9607269999999998E-7</v>
+      </c>
+    </row>
+    <row r="59" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B59">
         <v>9.5190199999999994</v>
       </c>
@@ -29300,6 +29763,22 @@
       </c>
       <c r="G59">
         <v>30.312632000000001</v>
+      </c>
+      <c r="I59">
+        <f>(B59-5)/1000</f>
+        <v>4.5190199999999995E-3</v>
+      </c>
+      <c r="J59">
+        <f t="shared" si="22"/>
+        <v>2.294403E-7</v>
+      </c>
+      <c r="M59">
+        <f t="shared" si="25"/>
+        <v>4.5429929999999995E-3</v>
+      </c>
+      <c r="N59">
+        <f t="shared" si="26"/>
+        <v>3.0312631999999998E-7</v>
       </c>
     </row>
   </sheetData>
@@ -35698,7 +36177,7 @@
         <v>-6.8636400000000002</v>
       </c>
       <c r="C12">
-        <f t="shared" ref="C3:C24" si="3">10^B12*100^2</f>
+        <f t="shared" ref="C12:C24" si="3">10^B12*100^2</f>
         <v>1.3688630479485528E-3</v>
       </c>
       <c r="E12">

</xml_diff>